<commit_message>
implement beta function and real beta values
</commit_message>
<xml_diff>
--- a/tx_dintéret_OAT.xlsx
+++ b/tx_dintéret_OAT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal_projects\Finance\DividendModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A7AC37-AF94-4358-A224-81CE40E91551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05BDE04-4710-48CB-A615-7CAFF4BB17D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="22080" yWindow="2040" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{582DEF8A-5162-4F84-B3CB-E1243C4765D2}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{582DEF8A-5162-4F84-B3CB-E1243C4765D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC609CD-7C71-4093-BB05-53C28FC320A8}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>